<commit_message>
edit & make model
</commit_message>
<xml_diff>
--- a/設計/Rr.wing/解析/迎角/データシート.xlsx
+++ b/設計/Rr.wing/解析/迎角/データシート.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ku_sk\Documents\Inventor\AeroCAD2018\CAD\Inventor\Aero Parts\R-wing\type7-naca97\解析用\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ku_sk\Documents\Inventor\AeroCAD2018\設計\Rr.wing\解析\迎角\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="19560" windowHeight="8055" tabRatio="875"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="19560" windowHeight="8055" tabRatio="875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-69D0-436C-BDDE-A69BAF854CCF}"/>
+              <c16:uniqueId val="{00000000-168D-49FA-8686-52F58C1C1745}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -562,7 +562,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-69D0-436C-BDDE-A69BAF854CCF}"/>
+              <c16:uniqueId val="{00000001-168D-49FA-8686-52F58C1C1745}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -685,7 +685,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-69D0-436C-BDDE-A69BAF854CCF}"/>
+              <c16:uniqueId val="{00000002-168D-49FA-8686-52F58C1C1745}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1583,21 +1583,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>537883</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>169207</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>88525</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>154641</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="グラフ 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1880,7 +1882,7 @@
   <dimension ref="B2:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>